<commit_message>
Se agrega el ícono pointer. Se cambia de nombre la carpeta BEL por BLUE y se deprecan los íconos de móvil para el proyecto de BLUE Banca Móvil.Iconos Version 2.6
</commit_message>
<xml_diff>
--- a/Iconos/Versiones/Mantenimiento Iconos 2.6.xlsx
+++ b/Iconos/Versiones/Mantenimiento Iconos 2.6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaramirez/Documents/GitHub/Icon-version/Iconos/Versiones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3A3FB5-BF57-6941-986F-8DB18157758D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CFB556-D36C-0C4E-B125-5941674C4A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" activeTab="15" xr2:uid="{1392F145-BFF9-584F-9FD8-96983AD39B37}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{1392F145-BFF9-584F-9FD8-96983AD39B37}"/>
   </bookViews>
   <sheets>
     <sheet name="Match inicial" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="2.3" sheetId="13" r:id="rId13"/>
     <sheet name="2.4" sheetId="14" r:id="rId14"/>
     <sheet name="2.5" sheetId="15" r:id="rId15"/>
-    <sheet name="Hoja1" sheetId="16" r:id="rId16"/>
+    <sheet name="2.6" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10530" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10536" uniqueCount="685">
   <si>
     <t>Clase App</t>
   </si>
@@ -2094,7 +2094,16 @@
     <t>clock-stk: e219</t>
   </si>
   <si>
-    <t>secured</t>
+    <t>e221</t>
+  </si>
+  <si>
+    <t>pointer</t>
+  </si>
+  <si>
+    <t>pointer: e221</t>
+  </si>
+  <si>
+    <t>Se agrega el ícono pointer. Se cambia de nombre la carpeta BEL por BLUE y se deprecan los íconos de móvil para el proyecto de BLUE Banca Móvil.</t>
   </si>
 </sst>
 </file>
@@ -21595,8 +21604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5DB87A-4193-9448-9B36-6817A16AFCD6}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="E206" sqref="E206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24722,13 +24731,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2321FE-5A2A-6D40-9A4E-8025D53A0466}">
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:E202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D204" sqref="D204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
@@ -24796,7 +24805,7 @@
         <v>375</v>
       </c>
       <c r="C4" s="142" t="s">
-        <v>681</v>
+        <v>408</v>
       </c>
       <c r="D4" s="143" t="s">
         <v>375</v>
@@ -27493,7 +27502,7 @@
       </c>
       <c r="E178" s="30"/>
     </row>
-    <row r="179" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="126" t="s">
         <v>626</v>
       </c>
@@ -27508,7 +27517,7 @@
       </c>
       <c r="E179" s="127"/>
     </row>
-    <row r="180" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="126" t="s">
         <v>628</v>
       </c>
@@ -27523,7 +27532,7 @@
       </c>
       <c r="E180" s="127"/>
     </row>
-    <row r="181" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="126" t="s">
         <v>630</v>
       </c>
@@ -27538,7 +27547,7 @@
       </c>
       <c r="E181" s="127"/>
     </row>
-    <row r="182" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="126" t="s">
         <v>632</v>
       </c>
@@ -27817,31 +27826,45 @@
       </c>
     </row>
     <row r="200" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A200" s="147" t="s">
+      <c r="A200" s="145" t="s">
         <v>679</v>
       </c>
-      <c r="B200" s="147" t="s">
+      <c r="B200" s="145" t="s">
         <v>675</v>
       </c>
-      <c r="C200" s="147" t="s">
+      <c r="C200" s="145" t="s">
         <v>679</v>
       </c>
-      <c r="D200" s="147" t="s">
+      <c r="D200" s="145" t="s">
         <v>675</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A201" s="147" t="s">
+      <c r="A201" s="145" t="s">
         <v>677</v>
       </c>
-      <c r="B201" s="147" t="s">
+      <c r="B201" s="145" t="s">
         <v>676</v>
       </c>
-      <c r="C201" s="147" t="s">
+      <c r="C201" s="145" t="s">
         <v>677</v>
       </c>
-      <c r="D201" s="147" t="s">
+      <c r="D201" s="145" t="s">
         <v>676</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A202" s="147" t="s">
+        <v>682</v>
+      </c>
+      <c r="B202" s="147" t="s">
+        <v>681</v>
+      </c>
+      <c r="C202" s="147" t="s">
+        <v>682</v>
+      </c>
+      <c r="D202" s="147" t="s">
+        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -27851,10 +27874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE09E71-EDDD-E849-BD57-A1E1F93BF035}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="B178" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28867,7 +28890,7 @@
     </row>
     <row r="163" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="154">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="B163" s="139" t="s">
         <v>269</v>
@@ -28887,8 +28910,23 @@
       </c>
       <c r="C165" s="139"/>
     </row>
+    <row r="166" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A166" s="154">
+        <v>2.6</v>
+      </c>
+      <c r="B166" s="139" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A167" s="154"/>
+      <c r="B167" s="139" t="s">
+        <v>683</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A166:A167"/>
     <mergeCell ref="A163:A165"/>
     <mergeCell ref="A141:A153"/>
     <mergeCell ref="A154:A157"/>

</xml_diff>